<commit_message>
LPF-960: code review comments and tidy-up LPF-960 - new pivot checks
LPF-960 - remove blank line added by mistake

LPF-960 - remove star import

LPF-960 - refactor to use streams to simplify

LPF-960 - clean up pivot exception formatting

LPF-960 - tighten up number conversions

LPF-960 - avoid forEach throwing exceptions

LPF-960 - avoid forEach throwing exceptions

LPF-960 - remove unused function

LPF-960 - cleanup some tests

LPF-960 - avoid internal function

LPF-960 - put back some old data

LPF-960 - put back some old data
</commit_message>
<xml_diff>
--- a/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
+++ b/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
@@ -1163,11 +1163,11 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45144.0</v>
+        <v>45651.0</v>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>CIS transaction</t>
+          <t>Invisibility potion</t>
         </is>
       </c>
       <c r="C2" s="5" t="n">
@@ -1190,7 +1190,7 @@
         <v>2.0</v>
       </c>
       <c r="D3" s="7" t="n">
-        <v>2.45</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>CIS transaction</t>
+          <t>Energy increase</t>
         </is>
       </c>
       <c r="C5" s="5" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>eForms</t>
+          <t>Extra energy increase</t>
         </is>
       </c>
       <c r="C6" s="5" t="n">

</xml_diff>

<commit_message>
LPF-960 - update CCMS invocie analysis data
LPF-960 - commit test

LPF-960 - undo commit test

LPF-960 - update expected response to have data
</commit_message>
<xml_diff>
--- a/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
+++ b/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="2"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
+    <sheet name="MAIN" r:id="rId9" sheetId="7"/>
+    <sheet name="CIS to CCMS import analysis" r:id="rId3" sheetId="1"/>
+    <sheet name="CIS to CCMS import exceptions" r:id="rId4" sheetId="2"/>
+    <sheet name="CCMS Payment value (user def)" r:id="rId5" sheetId="3"/>
+    <sheet name="CCMS Payment value (not def)" r:id="rId6" sheetId="4"/>
     <sheet name="CCMS Held payments" r:id="rId7" sheetId="5"/>
-    <sheet name="CIS to CCMS import exceptions" r:id="rId4" sheetId="2"/>
-    <sheet name="CIS to CCMS import analysis" r:id="rId3" sheetId="1"/>
-    <sheet name="CCMS Payment value(defined)" r:id="rId5" sheetId="3"/>
-    <sheet name="MAIN" r:id="rId9" sheetId="7"/>
-    <sheet name="CCMS Payment value(not defined)" r:id="rId6" sheetId="4"/>
     <sheet name="CCMS AP Debtors" r:id="rId8" sheetId="6"/>
   </sheets>
   <pivotCaches>
@@ -57,7 +57,9 @@
     <t>Analysis of HUB data transfers over the last 14 days</t>
   </si>
   <si>
-    <t>Please note the bulk of CWA contract payments are normaly only uploaded to CIS within the last few days of each month</t>
+    <t xml:space="preserve">Please note the bulk of CWA contract payments are normaly only uploaded to CIS within the last
+                        few days of each month
+                    </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -121,13 +123,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="dddd\ dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="dd-MMM-yy"/>
+    <numFmt numFmtId="165" formatCode="#.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="68">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -135,8 +139,193 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -144,42 +333,42 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -187,49 +376,49 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -237,7 +426,7 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -245,7 +434,7 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -253,56 +442,63 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -310,17 +506,38 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color theme="1"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
@@ -354,80 +571,256 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="15" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="40" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="43" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="50" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="52" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="right"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="164" fontId="16" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="166" fontId="53" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="right"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="17" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="54" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="42" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="166" fontId="22" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="23" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="167" fontId="55" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="56" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="58" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="168" fontId="60" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="61" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="left"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="24" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="62" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="42" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="26" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="63" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="169" fontId="64" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="65" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="169" fontId="67" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ dddd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ dddd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Jason Smallman" refreshedDate="45710.05277430556" createdVersion="7" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="2" refreshOnLoad="true">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshOnLoad="true" refreshedBy="Christopher Cook" refreshedDate="45861.74514050926" createdVersion="7" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="rId1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D1048576" sheet="CIS to CCMS import analysis"/>
   </cacheSource>
   <cacheFields count="4">
-    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="12" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-07-25T00:00:00" maxDate="2023-08-08T00:00:00">
+    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="20" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-07-25T00:00:00" maxDate="2023-08-17T00:00:00">
         <m/>
+        <d v="2023-08-07T00:00:00" u="1"/>
+        <d v="2023-08-08T00:00:00" u="1"/>
+        <d v="2023-08-09T00:00:00" u="1"/>
+        <d v="2023-08-10T00:00:00" u="1"/>
+        <d v="2023-08-11T00:00:00" u="1"/>
+        <d v="2023-08-15T00:00:00" u="1"/>
+        <d v="2023-08-03T00:00:00" u="1"/>
+        <d v="2023-08-04T00:00:00" u="1"/>
+        <d v="2023-08-06T00:00:00" u="1"/>
+        <d v="2023-08-14T00:00:00" u="1"/>
+        <d v="2023-08-16T00:00:00" u="1"/>
+        <d v="2023-08-13T00:00:00" u="1"/>
         <d v="2023-07-25T00:00:00" u="1"/>
         <d v="2023-08-02T00:00:00" u="1"/>
-        <d v="2023-08-07T00:00:00" u="1"/>
         <d v="2023-07-26T00:00:00" u="1"/>
         <d v="2023-07-27T00:00:00" u="1"/>
         <d v="2023-07-28T00:00:00" u="1"/>
         <d v="2023-07-31T00:00:00" u="1"/>
         <d v="2023-08-01T00:00:00" u="1"/>
-        <d v="2023-08-03T00:00:00" u="1"/>
-        <d v="2023-08-04T00:00:00" u="1"/>
-        <d v="2023-08-06T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="THE_SYSTEM" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="7" containsBlank="1" containsNonDate="0">
         <m/>
         <s v="CWA Crime Lower Contract" u="1"/>
-        <s v="CIS transaction" u="1"/>
         <s v="AGFS scheme" u="1"/>
         <s v="eForms" u="1"/>
         <s v="LGFS scheme" u="1"/>
+        <s v="CIS transaction" u="1"/>
         <s v="CWA Legal Help Contract" u="1"/>
       </sharedItems>
     </cacheField>
@@ -442,14 +835,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Jason Smallman" refreshedDate="45710.05277430556" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="3" refreshOnLoad="true">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshOnLoad="true" refreshedBy="Christopher Cook" refreshedDate="45861.7456912037" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" r:id="rId1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L7992" sheet="CIS to CCMS import exceptions"/>
+    <worksheetSource ref="A1:L1048576" sheet="CIS to CCMS import exceptions"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="ACC_CODE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="2" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-01-02T00:00:00" maxDate="2023-01-03T00:00:00">
+      <sharedItems count="3" containsBlank="1" containsDate="1" containsMixedTypes="1" containsNonDate="0" minDate="2023-01-02T00:00:00" maxDate="2023-01-03T00:00:00">
         <m/>
+        <s v="c" u="1"/>
         <d v="2023-01-02T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
@@ -462,10 +856,10 @@
     <cacheField name="THE_SYSTEM" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="DATE_CREATED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="DATE_CREATED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
     <cacheField name="TRANS_INT_ID" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
@@ -480,7 +874,7 @@
     <cacheField name="INVOICE_ID" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="GL_DATE" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="GL_DATE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
     <cacheField name="INVOICE_AMOUNT" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
@@ -503,30 +897,38 @@
   <location ref="A18:C21" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="ascending" defaultSubtotal="1">
-      <items count="13">
+      <items count="21">
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="9"/>
         <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" sd="1" m="1" x="4"/>
         <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="10"/>
         <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="10"/>
         <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
       <items count="8">
+        <item t="data" sd="1" m="1" x="5"/>
         <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="4"/>
         <item t="data" sd="1" m="1" x="1"/>
         <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" h="1" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
@@ -547,20 +949,20 @@
     <field x="-2"/>
   </colFields>
   <dataFields count="2">
-    <dataField name="CIS Value" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="5" numFmtId="165"/>
-    <dataField name="CCMS Value" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="4" numFmtId="165"/>
+    <dataField name="CIS Value" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="5" numFmtId="15"/>
+    <dataField name="CCMS Value" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="4" numFmtId="15"/>
   </dataFields>
-  <formats count="7">
-    <format action="formatting" dxfId="6">
+  <formats count="8">
+    <format action="formatting" dxfId="33">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="5">
+    <format action="formatting" dxfId="32">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format action="formatting" dxfId="4">
+    <format action="formatting" dxfId="31">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="3">
+    <format action="formatting" dxfId="30">
       <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294">
@@ -569,7 +971,7 @@
         </references>
       </pivotArea>
     </format>
-    <format action="formatting" dxfId="2">
+    <format action="formatting" dxfId="29">
       <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294">
@@ -578,10 +980,10 @@
         </references>
       </pivotArea>
     </format>
-    <format action="formatting" dxfId="1">
+    <format action="formatting" dxfId="28">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="0">
+    <format action="formatting" dxfId="27">
       <pivotArea type="normal" dataOnly="0" labelOnly="1" outline="1" fieldPosition="0">
         <references count="1">
           <reference field="0">
@@ -600,6 +1002,26 @@
         </references>
       </pivotArea>
     </format>
+    <format action="formatting" dxfId="26">
+      <pivotArea type="normal" dataOnly="0" labelOnly="1" outline="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0">
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="16"/>
+            <x v="17"/>
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
@@ -610,9 +1032,10 @@
   <location ref="A52:C55" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="3">
+      <items count="4">
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" x="0"/>
         <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
@@ -651,37 +1074,205 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="CIS Value" fld="8" subtotal="sum" showDataAs="normal" baseField="0" baseItem="2" numFmtId="165"/>
-    <dataField name="CCMS Value" fld="11" subtotal="sum" showDataAs="normal" baseField="0" baseItem="1" numFmtId="165"/>
+    <dataField name="CIS Value" fld="8" subtotal="sum" showDataAs="normal" baseField="0" baseItem="2" numFmtId="168"/>
+    <dataField name="CCMS Value" fld="11" subtotal="sum" showDataAs="normal" baseField="0" baseItem="1" numFmtId="168"/>
   </dataFields>
+  <formats count="4">
+    <format action="formatting" dxfId="25">
+      <pivotArea type="normal" dataOnly="1" outline="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="24">
+      <pivotArea type="normal" dataOnly="1" outline="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="23">
+      <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="22">
+      <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.66796875"/>
+    <col min="2" max="2" customWidth="true" width="22.828125"/>
+    <col min="3" max="3" customWidth="true" width="10.16796875"/>
+    <col min="4" max="4" customWidth="true" width="11.828125"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>DATE_AUTHORISED_CIS</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>THE_SYSTEM</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>CIS_VALUE</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>CCMS_VALUE</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="2" t="n">
+        <v>45144.0</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>CIS transaction</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="2" t="n">
+        <v>45140.0</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Healing spell</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>2.45</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="2" t="n">
+        <v>45140.0</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Headache cure</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="2" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>CIS transaction</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>10466.08</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>10466.08</v>
+      </c>
+    </row>
     <row r="6">
-</row>
+      <c r="A6" s="2" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>eForms</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1258037.63</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>1256489.69</v>
+      </c>
+    </row>
     <row r="7">
-</row>
+      <c r="A7" s="2" t="n">
+        <v>45133.0</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Nacho-flavoured headache cure</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>16231.76</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>16231.76</v>
+      </c>
+    </row>
     <row r="8">
-</row>
+      <c r="A8" s="2" t="n">
+        <v>45133.0</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>The Complete Wizard Potion Set</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>1345210.89</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>1345210.89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -689,16 +1280,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="9.328125"/>
+    <col min="2" max="2" customWidth="true" width="18.66796875"/>
+    <col min="3" max="3" customWidth="true" width="17.328125"/>
+    <col min="4" max="4" customWidth="true" width="11.16796875"/>
+    <col min="5" max="5" customWidth="true" width="17.16796875"/>
+    <col min="6" max="6" customWidth="true" width="20.66796875"/>
+    <col min="7" max="7" customWidth="true" width="12.66796875"/>
+    <col min="8" max="8" customWidth="true" width="7.66796875"/>
+    <col min="9" max="9" customWidth="true" width="9.16796875"/>
+    <col min="10" max="10" customWidth="true" width="10.0"/>
+    <col min="11" max="11" customWidth="true" width="7.66796875"/>
+    <col min="12" max="12" customWidth="true" width="16.5"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ACC_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>ACCO_HELD_BY_TYPE</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>DTYP_DOC_TYPE_ID</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>THE_SYSTEM</t>
+        </is>
+      </c>
+      <c r="E1" s="13" t="inlineStr">
+        <is>
+          <t>DATE_CREATED_CIS</t>
+        </is>
+      </c>
+      <c r="F1" s="15" t="inlineStr">
+        <is>
+          <t>DATE_AUTHORISED_CIS</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>TRANS_INT_ID</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>VOLUME</t>
+        </is>
+      </c>
+      <c r="I1" s="19" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>INVOICE_ID</t>
+        </is>
+      </c>
+      <c r="K1" s="22" t="inlineStr">
+        <is>
+          <t>GL_DATE</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>INVOICE_AMOUNT</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>02BZR</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>FL32</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Fluffy</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>In a bag</t>
+        </is>
+      </c>
+      <c r="E2" s="13" t="n">
+        <v>40444.0</v>
+      </c>
+      <c r="F2" s="15" t="n">
+        <v>45019.0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I2" s="19" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>5847847.0</v>
+      </c>
+      <c r="K2" s="22" t="n">
+        <v>44907.0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>42.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -706,16 +1415,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="63.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="9.16796875"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="27" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="29" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="31" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>A7373</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Cod On The Coast</t>
+        </is>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>45141.0</v>
+      </c>
+      <c r="D2" s="29" t="n">
+        <v>45142.0</v>
+      </c>
+      <c r="E2" s="31" t="n">
+        <v>3231.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -723,18 +1483,104 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="35.0"/>
+    <col min="3" max="3" customWidth="true" width="24.828125"/>
+    <col min="4" max="4" customWidth="true" width="13.328125"/>
+    <col min="5" max="5" customWidth="true" width="15.0"/>
+    <col min="6" max="6" customWidth="true" width="8.16796875"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>PAY_GROUP_LOOKUP_CODE</t>
+        </is>
+      </c>
+      <c r="D1" s="36" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="38" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="F1" s="40" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>LLDJ4214</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Chocolate fudge cake</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>CHOCOLATE</t>
+        </is>
+      </c>
+      <c r="D2" s="36" t="n">
+        <v>43077.0</v>
+      </c>
+      <c r="E2" s="38" t="n">
+        <v>43077.0</v>
+      </c>
+      <c r="F2" s="40" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>NNFDJ343</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Victoria sponge</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>SPONGE</t>
+        </is>
+      </c>
+      <c r="D3" s="36" t="n">
+        <v>44131.0</v>
+      </c>
+      <c r="E3" s="38" t="n">
+        <v>44131.0</v>
+      </c>
+      <c r="F3" s="40" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -742,36 +1588,277 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="68.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="21.0"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="44" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="46" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="48" t="inlineStr">
+        <is>
+          <t>TOTAL_INC_MEDIATION</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>1AA11A</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="C2" s="44" t="n">
+        <v>44645.0</v>
+      </c>
+      <c r="D2" s="46" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="E2" s="48" t="n">
+        <v>489695.61</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>1AA11B</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C3" s="44" t="n">
+        <v>42835.0</v>
+      </c>
+      <c r="D3" s="46" t="n">
+        <v>44893.0</v>
+      </c>
+      <c r="E3" s="48" t="n">
+        <v>352559.28</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>74ABBD</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Sinéad</t>
+        </is>
+      </c>
+      <c r="C4" s="44" t="n">
+        <v>41565.0</v>
+      </c>
+      <c r="D4" s="46" t="n">
+        <v>43873.0</v>
+      </c>
+      <c r="E4" s="48" t="n">
+        <v>242610.75</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>5544DS</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C5" s="44" t="n">
+        <v>45052.0</v>
+      </c>
+      <c r="D5" s="46" t="n">
+        <v>45083.0</v>
+      </c>
+      <c r="E5" s="48" t="n">
+        <v>234639.37</v>
+      </c>
+    </row>
     <row r="6">
-</row>
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>848dNDN</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Hellema</t>
+        </is>
+      </c>
+      <c r="C6" s="44" t="n">
+        <v>44643.0</v>
+      </c>
+      <c r="D6" s="46" t="n">
+        <v>45134.0</v>
+      </c>
+      <c r="E6" s="48" t="n">
+        <v>193722.84</v>
+      </c>
+    </row>
     <row r="7">
-</row>
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>JDJHF34</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>VID</t>
+        </is>
+      </c>
+      <c r="C7" s="44" t="n">
+        <v>41202.0</v>
+      </c>
+      <c r="D7" s="46" t="n">
+        <v>44624.0</v>
+      </c>
+      <c r="E7" s="48" t="n">
+        <v>140817.24</v>
+      </c>
+    </row>
     <row r="8">
-</row>
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>84KDSD</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Alan</t>
+        </is>
+      </c>
+      <c r="C8" s="44" t="n">
+        <v>43358.0</v>
+      </c>
+      <c r="D8" s="46" t="n">
+        <v>44187.0</v>
+      </c>
+      <c r="E8" s="48" t="n">
+        <v>111330.91</v>
+      </c>
+    </row>
     <row r="9">
-</row>
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>5DJFJ</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ISAAC</t>
+        </is>
+      </c>
+      <c r="C9" s="44" t="n">
+        <v>42961.0</v>
+      </c>
+      <c r="D9" s="46" t="n">
+        <v>44615.0</v>
+      </c>
+      <c r="E9" s="48" t="n">
+        <v>62318.93</v>
+      </c>
+    </row>
     <row r="10">
-</row>
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>43fFFDS</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+      <c r="C10" s="44" t="n">
+        <v>41950.0</v>
+      </c>
+      <c r="D10" s="46" t="n">
+        <v>42885.0</v>
+      </c>
+      <c r="E10" s="48" t="n">
+        <v>59135.36</v>
+      </c>
+    </row>
     <row r="11">
-</row>
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>4DFDDF</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>MARTY</t>
+        </is>
+      </c>
+      <c r="C11" s="44" t="n">
+        <v>45135.0</v>
+      </c>
+      <c r="D11" s="46" t="n">
+        <v>45135.0</v>
+      </c>
+      <c r="E11" s="48" t="n">
+        <v>54876.28</v>
+      </c>
+    </row>
     <row r="12">
-</row>
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>5JXJC</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>CJ</t>
+        </is>
+      </c>
+      <c r="C12" s="44" t="n">
+        <v>42685.0</v>
+      </c>
+      <c r="D12" s="46" t="n">
+        <v>43619.0</v>
+      </c>
+      <c r="E12" s="48" t="n">
+        <v>49186.71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -779,22 +1866,130 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="68.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="21.0"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="52" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="54" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="56" t="inlineStr">
+        <is>
+          <t>TOTAL_INC_MEDIATION</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>5430C</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>PJE</t>
+        </is>
+      </c>
+      <c r="C2" s="52" t="n">
+        <v>41212.0</v>
+      </c>
+      <c r="D2" s="54" t="n">
+        <v>44327.0</v>
+      </c>
+      <c r="E2" s="56" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>8932J</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>LAP</t>
+        </is>
+      </c>
+      <c r="C3" s="52" t="n">
+        <v>41249.0</v>
+      </c>
+      <c r="D3" s="54" t="n">
+        <v>42410.0</v>
+      </c>
+      <c r="E3" s="56" t="n">
+        <v>-2.0</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>9182F</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>DAS</t>
+        </is>
+      </c>
+      <c r="C4" s="52" t="n">
+        <v>41316.0</v>
+      </c>
+      <c r="D4" s="54" t="n">
+        <v>45076.0</v>
+      </c>
+      <c r="E4" s="56" t="n">
+        <v>-2.0</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>0P337X</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>SLB</t>
+        </is>
+      </c>
+      <c r="C5" s="52" t="n">
+        <v>41458.0</v>
+      </c>
+      <c r="D5" s="54" t="n">
+        <v>44186.0</v>
+      </c>
+      <c r="E5" s="56" t="n">
+        <v>-2394.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -811,17 +2006,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="true"/>
-    <col min="2" max="2" width="20.6640625" customWidth="true"/>
-    <col min="3" max="3" width="20.6640625" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="26.1640625"/>
+    <col min="2" max="2" customWidth="true" width="20.6640625"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="true" hidden="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
@@ -833,112 +2028,116 @@
       <c r="L1" s="0"/>
     </row>
     <row r="2" ht="15.0" customHeight="true" hidden="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
     </row>
     <row r="3" ht="16.0" customHeight="true" hidden="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
     </row>
     <row r="4" ht="16.0" customHeight="true" hidden="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" ht="15.0" customHeight="true" hidden="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
     </row>
     <row r="6" ht="15.0" customHeight="true" hidden="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true" hidden="false">
-      <c r="A7" s="14"/>
+      <c r="A7" s="70"/>
     </row>
     <row r="8" ht="15.0" customHeight="true" hidden="false">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="72" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="32.0" customHeight="true" hidden="false">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18">
-        <f>COUNTIF('CCMS Payment value(defined)'!E:E,"&gt;0")</f>
-      </c>
-      <c r="C9" s="19">
-        <f>SUM('CCMS Payment value(defined)'!E:E)</f>
+      <c r="B9" s="74">
+        <f>COUNTIF('CCMS Payment value (user def)'!E:E,"&gt;0")</f>
+      </c>
+      <c r="C9" s="75">
+        <f>SUM('CCMS Payment value (user def)'!E:E)</f>
       </c>
     </row>
     <row r="10" ht="32.0" customHeight="true" hidden="false">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18">
-        <f>COUNTIF('CCMS Payment value(not defined)'!F:F,"&gt;0")</f>
-      </c>
-      <c r="C10" s="19">
-        <f>SUM('CCMS Payment value(not defined)'!F:F)</f>
+      <c r="B10" s="74">
+        <f>COUNTIF('CCMS Payment value (not def)'!F:F,"&gt;0")</f>
+      </c>
+      <c r="C10" s="75">
+        <f>SUM('CCMS Payment value (not def)'!F:F)</f>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="true" hidden="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="74">
         <f>COUNTIF('CCMS Held payments'!E:E,"&gt;0")</f>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="75">
         <f>SUM('CCMS Held payments'!E:E)</f>
       </c>
     </row>
     <row r="12" ht="32.0" customHeight="true" hidden="true">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="74">
         <f>COUNTIF('CCMS AP Debtors'!E:E,"&lt;0")</f>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="75">
         <f>SUM('CCMS AP Debtors'!E:E)</f>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true" hidden="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="70" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="15.0" customHeight="true" hidden="false">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="76" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" ht="15.0" customHeight="true" hidden="false">
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="77"/>
+      <c r="B18" s="78" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" ht="15.0" customHeight="true" hidden="false"/>
+      <c r="C18" s="77"/>
+    </row>
+    <row r="19" ht="15.0" customHeight="true" hidden="false">
+      <c r="A19" s="77"/>
+    </row>
     <row r="20" ht="15.0" customHeight="true" hidden="false">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="79" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" ht="15.0" customHeight="true" hidden="false">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="80" t="s">
         <v>14</v>
       </c>
     </row>
@@ -957,138 +2156,140 @@
     <row r="34" ht="15.0" customHeight="true" hidden="false"/>
     <row r="35" ht="15.0" customHeight="true" hidden="false"/>
     <row r="37" ht="15.0" customHeight="true" hidden="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="75"/>
     </row>
     <row r="38" ht="15.0" customHeight="true" hidden="false">
-      <c r="A38" s="14"/>
+      <c r="A38" s="70"/>
     </row>
     <row r="39" ht="32.0" customHeight="true" hidden="false">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="81" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="40" ht="15.0" customHeight="true" hidden="false">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A40)</f>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A40,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="41" ht="15.0" customHeight="true" hidden="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A41)</f>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A41,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="42" ht="15.0" customHeight="true" hidden="false">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A42)</f>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A42,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="43" ht="15.0" customHeight="true" hidden="false">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A43)</f>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A43,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="44" ht="15.0" customHeight="true" hidden="false">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A44)</f>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A44,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="45" ht="15.0" customHeight="true" hidden="false">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A45)</f>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A45,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="46" ht="15.0" customHeight="true" hidden="false">
-      <c r="B46" s="18"/>
-      <c r="C46" s="25"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="83"/>
     </row>
     <row r="47" ht="15.0" customHeight="true" hidden="false">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="74">
         <f>SUM(B40:B46)</f>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="83">
         <f>SUM(C40:C46)</f>
       </c>
     </row>
     <row r="50" ht="15.0" customHeight="true" hidden="false">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="70" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="52" ht="15.0" customHeight="true" hidden="false">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="78" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" ht="15.0" customHeight="true" hidden="false">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="85" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="54" ht="15.0" customHeight="true" hidden="false">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="19"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="86"/>
     </row>
     <row r="55" ht="15.0" customHeight="true" hidden="false">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="19"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="86"/>
     </row>
     <row r="56" ht="15.0" customHeight="true" hidden="false"/>
     <row r="57" ht="15.0" customHeight="true" hidden="false"/>

</xml_diff>

<commit_message>
feature: LPF-960 - update AT coverage of pivot tables (#65)
* LPF-960 - update CCMS invocie analysis data

LPF-960 - commit test

LPF-960 - undo commit test

LPF-960 - update expected response to have data

* LPF-960: code review comments and tidy-up
LPF-960 - new pivot checks

LPF-960 - remove blank line added by mistake

LPF-960 - remove star import

LPF-960 - refactor to use streams to simplify

LPF-960 - clean up pivot exception formatting

LPF-960 - tighten up number conversions

LPF-960 - avoid forEach throwing exceptions

LPF-960 - avoid forEach throwing exceptions

LPF-960 - remove unused function

LPF-960 - cleanup some tests

LPF-960 - avoid internal function

LPF-960 - put back some old data

LPF-960 - put back some old data
</commit_message>
<xml_diff>
--- a/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
+++ b/src/test/resources/expected_results/CCMS Invoice Analysis (CIS to CCMS).xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="2"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
+    <sheet name="MAIN" r:id="rId9" sheetId="7"/>
+    <sheet name="CIS to CCMS import analysis" r:id="rId3" sheetId="1"/>
+    <sheet name="CIS to CCMS import exceptions" r:id="rId4" sheetId="2"/>
+    <sheet name="CCMS Payment value (user def)" r:id="rId5" sheetId="3"/>
+    <sheet name="CCMS Payment value (not def)" r:id="rId6" sheetId="4"/>
     <sheet name="CCMS Held payments" r:id="rId7" sheetId="5"/>
-    <sheet name="CIS to CCMS import exceptions" r:id="rId4" sheetId="2"/>
-    <sheet name="CIS to CCMS import analysis" r:id="rId3" sheetId="1"/>
-    <sheet name="CCMS Payment value(defined)" r:id="rId5" sheetId="3"/>
-    <sheet name="MAIN" r:id="rId9" sheetId="7"/>
-    <sheet name="CCMS Payment value(not defined)" r:id="rId6" sheetId="4"/>
     <sheet name="CCMS AP Debtors" r:id="rId8" sheetId="6"/>
   </sheets>
   <pivotCaches>
@@ -57,7 +57,9 @@
     <t>Analysis of HUB data transfers over the last 14 days</t>
   </si>
   <si>
-    <t>Please note the bulk of CWA contract payments are normaly only uploaded to CIS within the last few days of each month</t>
+    <t xml:space="preserve">Please note the bulk of CWA contract payments are normaly only uploaded to CIS within the last
+                        few days of each month
+                    </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -121,13 +123,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="dddd\ dd/mm/yyyy"/>
-    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="dd-MMM-yy"/>
+    <numFmt numFmtId="165" formatCode="#.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="68">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -135,8 +139,193 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -144,42 +333,42 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -187,49 +376,49 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -237,7 +426,7 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -245,7 +434,7 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -253,56 +442,63 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
-      <main:family val="2"/>
-      <main:color theme="1"/>
-      <main:sz val="11"/>
-      <main:scheme val="minor"/>
-    </font>
-    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
@@ -310,17 +506,38 @@
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:color theme="1"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
     <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <main:name val="Calibri"/>
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color theme="1"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
       <main:family val="2"/>
       <main:b val="1"/>
       <main:color theme="1"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
+      <main:sz val="11"/>
+      <main:scheme val="minor"/>
+    </font>
+    <font xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <main:name val="Aptos Narrow"/>
+      <main:family val="2"/>
+      <main:color indexed="8"/>
       <main:sz val="11"/>
       <main:scheme val="minor"/>
     </font>
@@ -354,80 +571,256 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="15" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="40" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="43" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="47" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="48" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="49" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="50" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="51" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="52" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="right"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="164" fontId="16" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="166" fontId="53" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="right"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="17" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="54" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="42" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf numFmtId="166" fontId="22" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="23" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="167" fontId="55" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="166" fontId="56" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="58" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="168" fontId="60" fillId="3" borderId="0" pivotButton="1" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="61" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="left"/>
     </xf>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="24" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="62" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="25" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="42" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
-    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="26" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="63" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
       <main:alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="169" fontId="64" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="65" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true">
+      <main:alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf numFmtId="169" fontId="67" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0" applyFill="true" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
+  <dxfs count="34">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ dddd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ dddd"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="dddd\ dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Jason Smallman" refreshedDate="45710.05277430556" createdVersion="7" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="2" refreshOnLoad="true">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshOnLoad="true" refreshedBy="Christopher Cook" refreshedDate="45861.74514050926" createdVersion="7" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="rId1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D1048576" sheet="CIS to CCMS import analysis"/>
   </cacheSource>
   <cacheFields count="4">
-    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="12" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-07-25T00:00:00" maxDate="2023-08-08T00:00:00">
+    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
+      <sharedItems count="20" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-07-25T00:00:00" maxDate="2023-08-17T00:00:00">
         <m/>
+        <d v="2023-08-07T00:00:00" u="1"/>
+        <d v="2023-08-08T00:00:00" u="1"/>
+        <d v="2023-08-09T00:00:00" u="1"/>
+        <d v="2023-08-10T00:00:00" u="1"/>
+        <d v="2023-08-11T00:00:00" u="1"/>
+        <d v="2023-08-15T00:00:00" u="1"/>
+        <d v="2023-08-03T00:00:00" u="1"/>
+        <d v="2023-08-04T00:00:00" u="1"/>
+        <d v="2023-08-06T00:00:00" u="1"/>
+        <d v="2023-08-14T00:00:00" u="1"/>
+        <d v="2023-08-16T00:00:00" u="1"/>
+        <d v="2023-08-13T00:00:00" u="1"/>
         <d v="2023-07-25T00:00:00" u="1"/>
         <d v="2023-08-02T00:00:00" u="1"/>
-        <d v="2023-08-07T00:00:00" u="1"/>
         <d v="2023-07-26T00:00:00" u="1"/>
         <d v="2023-07-27T00:00:00" u="1"/>
         <d v="2023-07-28T00:00:00" u="1"/>
         <d v="2023-07-31T00:00:00" u="1"/>
         <d v="2023-08-01T00:00:00" u="1"/>
-        <d v="2023-08-03T00:00:00" u="1"/>
-        <d v="2023-08-04T00:00:00" u="1"/>
-        <d v="2023-08-06T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="THE_SYSTEM" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="7" containsBlank="1" containsNonDate="0">
         <m/>
         <s v="CWA Crime Lower Contract" u="1"/>
-        <s v="CIS transaction" u="1"/>
         <s v="AGFS scheme" u="1"/>
         <s v="eForms" u="1"/>
         <s v="LGFS scheme" u="1"/>
+        <s v="CIS transaction" u="1"/>
         <s v="CWA Legal Help Contract" u="1"/>
       </sharedItems>
     </cacheField>
@@ -442,14 +835,15 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Jason Smallman" refreshedDate="45710.05277430556" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" r:id="3" refreshOnLoad="true">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshOnLoad="true" refreshedBy="Christopher Cook" refreshedDate="45861.7456912037" createdVersion="3" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" r:id="rId1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:L7992" sheet="CIS to CCMS import exceptions"/>
+    <worksheetSource ref="A1:L1048576" sheet="CIS to CCMS import exceptions"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="ACC_CODE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="2" containsBlank="1" containsDate="1" containsNonDate="0" containsString="0" minDate="2023-01-02T00:00:00" maxDate="2023-01-03T00:00:00">
+      <sharedItems count="3" containsBlank="1" containsDate="1" containsMixedTypes="1" containsNonDate="0" minDate="2023-01-02T00:00:00" maxDate="2023-01-03T00:00:00">
         <m/>
+        <s v="c" u="1"/>
         <d v="2023-01-02T00:00:00" u="1"/>
       </sharedItems>
     </cacheField>
@@ -462,10 +856,10 @@
     <cacheField name="THE_SYSTEM" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="DATE_CREATED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="DATE_CREATED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="DATE_AUTHORISED_CIS" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
     <cacheField name="TRANS_INT_ID" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
@@ -480,7 +874,7 @@
     <cacheField name="INVOICE_ID" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
-    <cacheField name="GL_DATE" uniqueList="1" numFmtId="15" sqlType="0" hierarchy="0" level="0" databaseField="1">
+    <cacheField name="GL_DATE" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
       <sharedItems count="0" containsBlank="1" containsNonDate="0" containsString="0"/>
     </cacheField>
     <cacheField name="INVOICE_AMOUNT" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
@@ -503,30 +897,38 @@
   <location ref="A18:C21" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="ascending" defaultSubtotal="1">
-      <items count="13">
+      <items count="21">
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="9"/>
         <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" sd="1" m="1" x="4"/>
         <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="10"/>
         <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="10"/>
         <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
       <items count="8">
+        <item t="data" sd="1" m="1" x="5"/>
         <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="4"/>
         <item t="data" sd="1" m="1" x="1"/>
         <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="3"/>
         <item t="data" h="1" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
@@ -547,20 +949,20 @@
     <field x="-2"/>
   </colFields>
   <dataFields count="2">
-    <dataField name="CIS Value" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="5" numFmtId="165"/>
-    <dataField name="CCMS Value" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="4" numFmtId="165"/>
+    <dataField name="CIS Value" fld="2" subtotal="sum" showDataAs="normal" baseField="0" baseItem="5" numFmtId="15"/>
+    <dataField name="CCMS Value" fld="3" subtotal="sum" showDataAs="normal" baseField="0" baseItem="4" numFmtId="15"/>
   </dataFields>
-  <formats count="7">
-    <format action="formatting" dxfId="6">
+  <formats count="8">
+    <format action="formatting" dxfId="33">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="5">
+    <format action="formatting" dxfId="32">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format action="formatting" dxfId="4">
+    <format action="formatting" dxfId="31">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="3">
+    <format action="formatting" dxfId="30">
       <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294">
@@ -569,7 +971,7 @@
         </references>
       </pivotArea>
     </format>
-    <format action="formatting" dxfId="2">
+    <format action="formatting" dxfId="29">
       <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294">
@@ -578,10 +980,10 @@
         </references>
       </pivotArea>
     </format>
-    <format action="formatting" dxfId="1">
+    <format action="formatting" dxfId="28">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format action="formatting" dxfId="0">
+    <format action="formatting" dxfId="27">
       <pivotArea type="normal" dataOnly="0" labelOnly="1" outline="1" fieldPosition="0">
         <references count="1">
           <reference field="0">
@@ -600,6 +1002,26 @@
         </references>
       </pivotArea>
     </format>
+    <format action="formatting" dxfId="26">
+      <pivotArea type="normal" dataOnly="0" labelOnly="1" outline="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0">
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+            <x v="11"/>
+            <x v="12"/>
+            <x v="13"/>
+            <x v="14"/>
+            <x v="15"/>
+            <x v="16"/>
+            <x v="17"/>
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
@@ -610,9 +1032,10 @@
   <location ref="A52:C55" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField axis="axisRow" showDropDowns="1" compact="1" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="3">
+      <items count="4">
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" x="0"/>
         <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" x="0"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
@@ -651,37 +1074,205 @@
     </i>
   </colItems>
   <dataFields count="2">
-    <dataField name="CIS Value" fld="8" subtotal="sum" showDataAs="normal" baseField="0" baseItem="2" numFmtId="165"/>
-    <dataField name="CCMS Value" fld="11" subtotal="sum" showDataAs="normal" baseField="0" baseItem="1" numFmtId="165"/>
+    <dataField name="CIS Value" fld="8" subtotal="sum" showDataAs="normal" baseField="0" baseItem="2" numFmtId="168"/>
+    <dataField name="CCMS Value" fld="11" subtotal="sum" showDataAs="normal" baseField="0" baseItem="1" numFmtId="168"/>
   </dataFields>
+  <formats count="4">
+    <format action="formatting" dxfId="25">
+      <pivotArea type="normal" dataOnly="1" outline="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="24">
+      <pivotArea type="normal" dataOnly="1" outline="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="23">
+      <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format action="formatting" dxfId="22">
+      <pivotArea type="normal" dataOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.66796875"/>
+    <col min="2" max="2" customWidth="true" width="22.828125"/>
+    <col min="3" max="3" customWidth="true" width="10.16796875"/>
+    <col min="4" max="4" customWidth="true" width="11.828125"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>DATE_AUTHORISED_CIS</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>THE_SYSTEM</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>CIS_VALUE</t>
+        </is>
+      </c>
+      <c r="D1" s="7" t="inlineStr">
+        <is>
+          <t>CCMS_VALUE</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="2" t="n">
+        <v>45651.0</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Invisibility potion</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="2" t="n">
+        <v>45140.0</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Healing spell</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="2" t="n">
+        <v>45140.0</v>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Headache cure</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="7" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="2" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Energy increase</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>10466.08</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>10466.08</v>
+      </c>
+    </row>
     <row r="6">
-</row>
+      <c r="A6" s="2" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Extra energy increase</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1258037.63</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>1256489.69</v>
+      </c>
+    </row>
     <row r="7">
-</row>
+      <c r="A7" s="2" t="n">
+        <v>45133.0</v>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Nacho-flavoured headache cure</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>16231.76</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>16231.76</v>
+      </c>
+    </row>
     <row r="8">
-</row>
+      <c r="A8" s="2" t="n">
+        <v>45133.0</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>The Complete Wizard Potion Set</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>1345210.89</v>
+      </c>
+      <c r="D8" s="7" t="n">
+        <v>1345210.89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -689,16 +1280,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="9.328125"/>
+    <col min="2" max="2" customWidth="true" width="18.66796875"/>
+    <col min="3" max="3" customWidth="true" width="17.328125"/>
+    <col min="4" max="4" customWidth="true" width="11.16796875"/>
+    <col min="5" max="5" customWidth="true" width="17.16796875"/>
+    <col min="6" max="6" customWidth="true" width="20.66796875"/>
+    <col min="7" max="7" customWidth="true" width="12.66796875"/>
+    <col min="8" max="8" customWidth="true" width="7.66796875"/>
+    <col min="9" max="9" customWidth="true" width="9.16796875"/>
+    <col min="10" max="10" customWidth="true" width="10.0"/>
+    <col min="11" max="11" customWidth="true" width="7.66796875"/>
+    <col min="12" max="12" customWidth="true" width="16.5"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ACC_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>ACCO_HELD_BY_TYPE</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>DTYP_DOC_TYPE_ID</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>THE_SYSTEM</t>
+        </is>
+      </c>
+      <c r="E1" s="13" t="inlineStr">
+        <is>
+          <t>DATE_CREATED_CIS</t>
+        </is>
+      </c>
+      <c r="F1" s="15" t="inlineStr">
+        <is>
+          <t>DATE_AUTHORISED_CIS</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>TRANS_INT_ID</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>VOLUME</t>
+        </is>
+      </c>
+      <c r="I1" s="19" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>INVOICE_ID</t>
+        </is>
+      </c>
+      <c r="K1" s="22" t="inlineStr">
+        <is>
+          <t>GL_DATE</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>INVOICE_AMOUNT</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>02BZR</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>FL32</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Fluffy</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>In a bag</t>
+        </is>
+      </c>
+      <c r="E2" s="13" t="n">
+        <v>40444.0</v>
+      </c>
+      <c r="F2" s="15" t="n">
+        <v>45019.0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="I2" s="19" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>5847847.0</v>
+      </c>
+      <c r="K2" s="22" t="n">
+        <v>44907.0</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>42.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -706,16 +1415,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="63.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="9.16796875"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="27" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="29" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="31" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>A7373</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Cod On The Coast</t>
+        </is>
+      </c>
+      <c r="C2" s="27" t="n">
+        <v>45141.0</v>
+      </c>
+      <c r="D2" s="29" t="n">
+        <v>45142.0</v>
+      </c>
+      <c r="E2" s="31" t="n">
+        <v>3231.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -723,18 +1483,104 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="35.0"/>
+    <col min="3" max="3" customWidth="true" width="24.828125"/>
+    <col min="4" max="4" customWidth="true" width="13.328125"/>
+    <col min="5" max="5" customWidth="true" width="15.0"/>
+    <col min="6" max="6" customWidth="true" width="8.16796875"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>PAY_GROUP_LOOKUP_CODE</t>
+        </is>
+      </c>
+      <c r="D1" s="36" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="38" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="F1" s="40" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>LLDJ4214</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Chocolate fudge cake</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>CHOCOLATE</t>
+        </is>
+      </c>
+      <c r="D2" s="36" t="n">
+        <v>43077.0</v>
+      </c>
+      <c r="E2" s="38" t="n">
+        <v>43077.0</v>
+      </c>
+      <c r="F2" s="40" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>NNFDJ343</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Victoria sponge</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>SPONGE</t>
+        </is>
+      </c>
+      <c r="D3" s="36" t="n">
+        <v>44131.0</v>
+      </c>
+      <c r="E3" s="38" t="n">
+        <v>44131.0</v>
+      </c>
+      <c r="F3" s="40" t="n">
+        <v>5.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -742,36 +1588,277 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="68.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="21.0"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="44" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="46" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="48" t="inlineStr">
+        <is>
+          <t>TOTAL_INC_MEDIATION</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>1AA11A</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Martin</t>
+        </is>
+      </c>
+      <c r="C2" s="44" t="n">
+        <v>44645.0</v>
+      </c>
+      <c r="D2" s="46" t="n">
+        <v>45145.0</v>
+      </c>
+      <c r="E2" s="48" t="n">
+        <v>489695.61</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>1AA11B</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Lucy</t>
+        </is>
+      </c>
+      <c r="C3" s="44" t="n">
+        <v>42835.0</v>
+      </c>
+      <c r="D3" s="46" t="n">
+        <v>44893.0</v>
+      </c>
+      <c r="E3" s="48" t="n">
+        <v>352559.28</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>74ABBD</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Sinéad</t>
+        </is>
+      </c>
+      <c r="C4" s="44" t="n">
+        <v>41565.0</v>
+      </c>
+      <c r="D4" s="46" t="n">
+        <v>43873.0</v>
+      </c>
+      <c r="E4" s="48" t="n">
+        <v>242610.75</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>5544DS</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Robert</t>
+        </is>
+      </c>
+      <c r="C5" s="44" t="n">
+        <v>45052.0</v>
+      </c>
+      <c r="D5" s="46" t="n">
+        <v>45083.0</v>
+      </c>
+      <c r="E5" s="48" t="n">
+        <v>234639.37</v>
+      </c>
+    </row>
     <row r="6">
-</row>
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>848dNDN</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Hellema</t>
+        </is>
+      </c>
+      <c r="C6" s="44" t="n">
+        <v>44643.0</v>
+      </c>
+      <c r="D6" s="46" t="n">
+        <v>45134.0</v>
+      </c>
+      <c r="E6" s="48" t="n">
+        <v>193722.84</v>
+      </c>
+    </row>
     <row r="7">
-</row>
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>JDJHF34</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>VID</t>
+        </is>
+      </c>
+      <c r="C7" s="44" t="n">
+        <v>41202.0</v>
+      </c>
+      <c r="D7" s="46" t="n">
+        <v>44624.0</v>
+      </c>
+      <c r="E7" s="48" t="n">
+        <v>140817.24</v>
+      </c>
+    </row>
     <row r="8">
-</row>
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>84KDSD</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Alan</t>
+        </is>
+      </c>
+      <c r="C8" s="44" t="n">
+        <v>43358.0</v>
+      </c>
+      <c r="D8" s="46" t="n">
+        <v>44187.0</v>
+      </c>
+      <c r="E8" s="48" t="n">
+        <v>111330.91</v>
+      </c>
+    </row>
     <row r="9">
-</row>
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>5DJFJ</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>ISAAC</t>
+        </is>
+      </c>
+      <c r="C9" s="44" t="n">
+        <v>42961.0</v>
+      </c>
+      <c r="D9" s="46" t="n">
+        <v>44615.0</v>
+      </c>
+      <c r="E9" s="48" t="n">
+        <v>62318.93</v>
+      </c>
+    </row>
     <row r="10">
-</row>
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>43fFFDS</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+      <c r="C10" s="44" t="n">
+        <v>41950.0</v>
+      </c>
+      <c r="D10" s="46" t="n">
+        <v>42885.0</v>
+      </c>
+      <c r="E10" s="48" t="n">
+        <v>59135.36</v>
+      </c>
+    </row>
     <row r="11">
-</row>
+      <c r="A11" s="0" t="inlineStr">
+        <is>
+          <t>4DFDDF</t>
+        </is>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>MARTY</t>
+        </is>
+      </c>
+      <c r="C11" s="44" t="n">
+        <v>45135.0</v>
+      </c>
+      <c r="D11" s="46" t="n">
+        <v>45135.0</v>
+      </c>
+      <c r="E11" s="48" t="n">
+        <v>54876.28</v>
+      </c>
+    </row>
     <row r="12">
-</row>
+      <c r="A12" s="0" t="inlineStr">
+        <is>
+          <t>5JXJC</t>
+        </is>
+      </c>
+      <c r="B12" s="0" t="inlineStr">
+        <is>
+          <t>CJ</t>
+        </is>
+      </c>
+      <c r="C12" s="44" t="n">
+        <v>42685.0</v>
+      </c>
+      <c r="D12" s="46" t="n">
+        <v>43619.0</v>
+      </c>
+      <c r="E12" s="48" t="n">
+        <v>49186.71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -779,22 +1866,130 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="17.828125"/>
+    <col min="2" max="2" customWidth="true" width="68.66796875"/>
+    <col min="3" max="3" customWidth="true" width="13.328125"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
+    <col min="5" max="5" customWidth="true" width="21.0"/>
+  </cols>
   <sheetData>
     <row r="1">
-</row>
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_CODE</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>VENDOR_SITE_NAME</t>
+        </is>
+      </c>
+      <c r="C1" s="52" t="inlineStr">
+        <is>
+          <t>FIRST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="D1" s="54" t="inlineStr">
+        <is>
+          <t>LATEST_GL_DATE</t>
+        </is>
+      </c>
+      <c r="E1" s="56" t="inlineStr">
+        <is>
+          <t>TOTAL_INC_MEDIATION</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
-</row>
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>5430C</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>PJE</t>
+        </is>
+      </c>
+      <c r="C2" s="52" t="n">
+        <v>41212.0</v>
+      </c>
+      <c r="D2" s="54" t="n">
+        <v>44327.0</v>
+      </c>
+      <c r="E2" s="56" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
     <row r="3">
-</row>
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>8932J</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>LAP</t>
+        </is>
+      </c>
+      <c r="C3" s="52" t="n">
+        <v>41249.0</v>
+      </c>
+      <c r="D3" s="54" t="n">
+        <v>42410.0</v>
+      </c>
+      <c r="E3" s="56" t="n">
+        <v>-2.0</v>
+      </c>
+    </row>
     <row r="4">
-</row>
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>9182F</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>DAS</t>
+        </is>
+      </c>
+      <c r="C4" s="52" t="n">
+        <v>41316.0</v>
+      </c>
+      <c r="D4" s="54" t="n">
+        <v>45076.0</v>
+      </c>
+      <c r="E4" s="56" t="n">
+        <v>-2.0</v>
+      </c>
+    </row>
     <row r="5">
-</row>
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>0P337X</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>SLB</t>
+        </is>
+      </c>
+      <c r="C5" s="52" t="n">
+        <v>41458.0</v>
+      </c>
+      <c r="D5" s="54" t="n">
+        <v>44186.0</v>
+      </c>
+      <c r="E5" s="56" t="n">
+        <v>-2394.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -811,17 +2006,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" customWidth="true"/>
-    <col min="2" max="2" width="20.6640625" customWidth="true"/>
-    <col min="3" max="3" width="20.6640625" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="26.1640625"/>
+    <col min="2" max="2" customWidth="true" width="20.6640625"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="true" hidden="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="59"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
@@ -833,112 +2028,116 @@
       <c r="L1" s="0"/>
     </row>
     <row r="2" ht="15.0" customHeight="true" hidden="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="62"/>
     </row>
     <row r="3" ht="16.0" customHeight="true" hidden="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
     </row>
     <row r="4" ht="16.0" customHeight="true" hidden="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" ht="15.0" customHeight="true" hidden="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69"/>
     </row>
     <row r="6" ht="15.0" customHeight="true" hidden="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="70" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="true" hidden="false">
-      <c r="A7" s="14"/>
+      <c r="A7" s="70"/>
     </row>
     <row r="8" ht="15.0" customHeight="true" hidden="false">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="72" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="32.0" customHeight="true" hidden="false">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18">
-        <f>COUNTIF('CCMS Payment value(defined)'!E:E,"&gt;0")</f>
-      </c>
-      <c r="C9" s="19">
-        <f>SUM('CCMS Payment value(defined)'!E:E)</f>
+      <c r="B9" s="74">
+        <f>COUNTIF('CCMS Payment value (user def)'!E:E,"&gt;0")</f>
+      </c>
+      <c r="C9" s="75">
+        <f>SUM('CCMS Payment value (user def)'!E:E)</f>
       </c>
     </row>
     <row r="10" ht="32.0" customHeight="true" hidden="false">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18">
-        <f>COUNTIF('CCMS Payment value(not defined)'!F:F,"&gt;0")</f>
-      </c>
-      <c r="C10" s="19">
-        <f>SUM('CCMS Payment value(not defined)'!F:F)</f>
+      <c r="B10" s="74">
+        <f>COUNTIF('CCMS Payment value (not def)'!F:F,"&gt;0")</f>
+      </c>
+      <c r="C10" s="75">
+        <f>SUM('CCMS Payment value (not def)'!F:F)</f>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="true" hidden="false">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="74">
         <f>COUNTIF('CCMS Held payments'!E:E,"&gt;0")</f>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="75">
         <f>SUM('CCMS Held payments'!E:E)</f>
       </c>
     </row>
     <row r="12" ht="32.0" customHeight="true" hidden="true">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="74">
         <f>COUNTIF('CCMS AP Debtors'!E:E,"&lt;0")</f>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="75">
         <f>SUM('CCMS AP Debtors'!E:E)</f>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="true" hidden="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="70" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="15.0" customHeight="true" hidden="false">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="76" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" ht="15.0" customHeight="true" hidden="false">
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="77"/>
+      <c r="B18" s="78" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" ht="15.0" customHeight="true" hidden="false"/>
+      <c r="C18" s="77"/>
+    </row>
+    <row r="19" ht="15.0" customHeight="true" hidden="false">
+      <c r="A19" s="77"/>
+    </row>
     <row r="20" ht="15.0" customHeight="true" hidden="false">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="79" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" ht="15.0" customHeight="true" hidden="false">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="80" t="s">
         <v>14</v>
       </c>
     </row>
@@ -957,138 +2156,140 @@
     <row r="34" ht="15.0" customHeight="true" hidden="false"/>
     <row r="35" ht="15.0" customHeight="true" hidden="false"/>
     <row r="37" ht="15.0" customHeight="true" hidden="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="75"/>
     </row>
     <row r="38" ht="15.0" customHeight="true" hidden="false">
-      <c r="A38" s="14"/>
+      <c r="A38" s="70"/>
     </row>
     <row r="39" ht="32.0" customHeight="true" hidden="false">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="81" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="40" ht="15.0" customHeight="true" hidden="false">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A40)</f>
       </c>
-      <c r="C40" s="25">
+      <c r="C40" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A40,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="41" ht="15.0" customHeight="true" hidden="false">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A41)</f>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A41,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="42" ht="15.0" customHeight="true" hidden="false">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A42)</f>
       </c>
-      <c r="C42" s="25">
+      <c r="C42" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A42,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="43" ht="15.0" customHeight="true" hidden="false">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="18">
+      <c r="B43" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A43)</f>
       </c>
-      <c r="C43" s="25">
+      <c r="C43" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A43,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="44" ht="15.0" customHeight="true" hidden="false">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="18">
+      <c r="B44" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A44)</f>
       </c>
-      <c r="C44" s="25">
+      <c r="C44" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A44,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="45" ht="15.0" customHeight="true" hidden="false">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B45" s="74">
         <f>COUNTIF('CIS to CCMS import exceptions'!D:D,A45)</f>
       </c>
-      <c r="C45" s="25">
+      <c r="C45" s="83">
         <f>SUMIF('CIS to CCMS import exceptions'!D:D,A45,'CIS to CCMS import exceptions'!I:I)</f>
       </c>
     </row>
     <row r="46" ht="15.0" customHeight="true" hidden="false">
-      <c r="B46" s="18"/>
-      <c r="C46" s="25"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="83"/>
     </row>
     <row r="47" ht="15.0" customHeight="true" hidden="false">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B47" s="74">
         <f>SUM(B40:B46)</f>
       </c>
-      <c r="C47" s="25">
+      <c r="C47" s="83">
         <f>SUM(C40:C46)</f>
       </c>
     </row>
     <row r="50" ht="15.0" customHeight="true" hidden="false">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="70" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="52" ht="15.0" customHeight="true" hidden="false">
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="78" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" ht="15.0" customHeight="true" hidden="false">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="85" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="54" ht="15.0" customHeight="true" hidden="false">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B54" s="19"/>
+      <c r="B54" s="86"/>
+      <c r="C54" s="86"/>
     </row>
     <row r="55" ht="15.0" customHeight="true" hidden="false">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="19"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="86"/>
     </row>
     <row r="56" ht="15.0" customHeight="true" hidden="false"/>
     <row r="57" ht="15.0" customHeight="true" hidden="false"/>

</xml_diff>